<commit_message>
new movie package(getWhen issue)
</commit_message>
<xml_diff>
--- a/CrowdSourcingStudy/Results/Second Study/Data/Dom_Sub/calculs_statistics(dom).xlsx
+++ b/CrowdSourcingStudy/Results/Second Study/Data/Dom_Sub/calculs_statistics(dom).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="19440" windowHeight="7140" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="450" windowWidth="19440" windowHeight="7140" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dominant" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
@@ -240,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,10 +256,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -271,11 +268,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,8 +286,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,6 +346,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -403,7 +413,7 @@
             <c:numRef>
               <c:f>principe1!$B$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.5714285714285716</c:v>
@@ -457,7 +467,7 @@
             <c:numRef>
               <c:f>principe1!$H$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.25</c:v>
@@ -521,7 +531,7 @@
             <c:numRef>
               <c:f>principe1!$E$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2.7142857142857144</c:v>
@@ -539,11 +549,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="974615040"/>
-        <c:axId val="970429504"/>
+        <c:axId val="960511488"/>
+        <c:axId val="960577536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="974615040"/>
+        <c:axId val="960511488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,7 +562,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="970429504"/>
+        <c:crossAx val="960577536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -560,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="970429504"/>
+        <c:axId val="960577536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -569,11 +579,11 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="974615040"/>
+        <c:crossAx val="960511488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -581,6 +591,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -632,6 +643,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -698,7 +710,7 @@
             <c:numRef>
               <c:f>principe1!$C$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2.7142857142857144</c:v>
@@ -747,7 +759,7 @@
             <c:numRef>
               <c:f>principe1!$I$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.9375</c:v>
@@ -782,7 +794,7 @@
             <c:numRef>
               <c:f>principe1!$F$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.5714285714285716</c:v>
@@ -800,11 +812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="976541696"/>
-        <c:axId val="970431808"/>
+        <c:axId val="48305664"/>
+        <c:axId val="960579840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="976541696"/>
+        <c:axId val="48305664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +825,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="970431808"/>
+        <c:crossAx val="960579840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="970431808"/>
+        <c:axId val="960579840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -830,11 +842,11 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="976541696"/>
+        <c:crossAx val="48305664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -842,6 +854,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -909,6 +922,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -975,7 +989,7 @@
             <c:numRef>
               <c:f>principe2!$B$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2.5416666666666665</c:v>
@@ -1024,7 +1038,7 @@
             <c:numRef>
               <c:f>principe2!$H$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.6875</c:v>
@@ -1083,7 +1097,7 @@
             <c:numRef>
               <c:f>principe2!$E$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.1428571428571428</c:v>
@@ -1101,11 +1115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="997880832"/>
-        <c:axId val="973270976"/>
+        <c:axId val="48307712"/>
+        <c:axId val="960582144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="997880832"/>
+        <c:axId val="48307712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="973270976"/>
+        <c:crossAx val="960582144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="973270976"/>
+        <c:axId val="960582144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1130,11 +1144,11 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="997880832"/>
+        <c:crossAx val="48307712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1143,6 +1157,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1210,6 +1225,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -1276,7 +1292,7 @@
             <c:numRef>
               <c:f>principe2!$C$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.8571428571428572</c:v>
@@ -1325,7 +1341,7 @@
             <c:numRef>
               <c:f>principe2!$I$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.6875</c:v>
@@ -1384,7 +1400,7 @@
             <c:numRef>
               <c:f>principe2!$F$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2.5714285714285716</c:v>
@@ -1402,11 +1418,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1003016192"/>
-        <c:axId val="973273280"/>
+        <c:axId val="48436224"/>
+        <c:axId val="960584448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1003016192"/>
+        <c:axId val="48436224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="973273280"/>
+        <c:crossAx val="960584448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1423,7 +1439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="973273280"/>
+        <c:axId val="960584448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1431,11 +1447,11 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1003016192"/>
+        <c:crossAx val="48436224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1450,6 +1466,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1711,11 +1728,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="976542720"/>
-        <c:axId val="976979072"/>
+        <c:axId val="48307200"/>
+        <c:axId val="514311296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="976542720"/>
+        <c:axId val="48307200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1724,7 +1741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="976979072"/>
+        <c:crossAx val="514311296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1732,7 +1749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="976979072"/>
+        <c:axId val="514311296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1751,7 +1768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="976542720"/>
+        <c:crossAx val="48307200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2006,11 +2023,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1007411200"/>
-        <c:axId val="976981952"/>
+        <c:axId val="960671744"/>
+        <c:axId val="514313600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1007411200"/>
+        <c:axId val="960671744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2019,7 +2036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="976981952"/>
+        <c:crossAx val="514313600"/>
         <c:crossesAt val="0.1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2027,7 +2044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="976981952"/>
+        <c:axId val="514313600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2040,7 +2057,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1007411200"/>
+        <c:crossAx val="960671744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2571,28 +2588,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="27"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2926,28 +2943,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="27"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -3229,28 +3246,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="C3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="27"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -3632,28 +3649,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="27"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -3914,28 +3931,28 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="27"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
@@ -4196,28 +4213,28 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
+      <c r="B33" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="27"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -4600,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4613,18 +4630,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="27"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -4659,10 +4676,10 @@
       <c r="F3" s="5">
         <v>4</v>
       </c>
-      <c r="H3" s="21">
-        <v>4</v>
-      </c>
-      <c r="I3" s="21">
+      <c r="H3" s="19">
+        <v>4</v>
+      </c>
+      <c r="I3" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4679,10 +4696,10 @@
       <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="H4" s="21">
-        <v>4</v>
-      </c>
-      <c r="I4" s="21">
+      <c r="H4" s="19">
+        <v>4</v>
+      </c>
+      <c r="I4" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4699,10 +4716,10 @@
       <c r="F5" s="5">
         <v>4</v>
       </c>
-      <c r="H5" s="21">
-        <v>5</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="H5" s="19">
+        <v>5</v>
+      </c>
+      <c r="I5" s="19">
         <v>2</v>
       </c>
     </row>
@@ -4719,10 +4736,10 @@
       <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="H6" s="21">
-        <v>1</v>
-      </c>
-      <c r="I6" s="21">
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19">
         <v>5</v>
       </c>
     </row>
@@ -4739,10 +4756,10 @@
       <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="H7" s="21">
-        <v>5</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="19">
         <v>5</v>
       </c>
     </row>
@@ -4759,10 +4776,10 @@
       <c r="F8" s="5">
         <v>4</v>
       </c>
-      <c r="H8" s="21">
-        <v>4</v>
-      </c>
-      <c r="I8" s="21">
+      <c r="H8" s="19">
+        <v>4</v>
+      </c>
+      <c r="I8" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4779,10 +4796,10 @@
       <c r="F9" s="5">
         <v>2</v>
       </c>
-      <c r="H9" s="21">
-        <v>4</v>
-      </c>
-      <c r="I9" s="21">
+      <c r="H9" s="19">
+        <v>4</v>
+      </c>
+      <c r="I9" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4791,10 +4808,10 @@
       <c r="C10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="H10" s="21">
-        <v>2</v>
-      </c>
-      <c r="I10" s="21">
+      <c r="H10" s="19">
+        <v>2</v>
+      </c>
+      <c r="I10" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4803,26 +4820,26 @@
       <c r="C11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="H11" s="21">
-        <v>4</v>
-      </c>
-      <c r="I11" s="21">
+      <c r="H11" s="19">
+        <v>4</v>
+      </c>
+      <c r="I11" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="21">
-        <v>4</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="H12" s="19">
+        <v>4</v>
+      </c>
+      <c r="I12" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="21">
-        <v>2</v>
-      </c>
-      <c r="I13" s="21">
+      <c r="H13" s="19">
+        <v>2</v>
+      </c>
+      <c r="I13" s="19">
         <v>4</v>
       </c>
     </row>
@@ -4831,42 +4848,42 @@
         <f>LOI.NORMALE.</f>
         <v>#NAME?</v>
       </c>
-      <c r="H14" s="21">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21">
+      <c r="H14" s="19">
+        <v>1</v>
+      </c>
+      <c r="I14" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="21">
-        <v>4</v>
-      </c>
-      <c r="I15" s="21">
+      <c r="H15" s="19">
+        <v>4</v>
+      </c>
+      <c r="I15" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="21">
-        <v>1</v>
-      </c>
-      <c r="I16" s="21">
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="21">
-        <v>3</v>
-      </c>
-      <c r="I17" s="21">
+      <c r="H17" s="19">
+        <v>3</v>
+      </c>
+      <c r="I17" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="21">
-        <v>4</v>
-      </c>
-      <c r="I18" s="21">
+      <c r="H18" s="19">
+        <v>4</v>
+      </c>
+      <c r="I18" s="19">
         <v>2</v>
       </c>
     </row>
@@ -4874,29 +4891,29 @@
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <f>AVERAGE(B3:B9)</f>
         <v>3.5714285714285716</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <f>AVERAGE(C3:C9)</f>
         <v>2.7142857142857144</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="22">
+      <c r="D20" s="22"/>
+      <c r="E20" s="21">
         <f>AVERAGE(E3:E9)</f>
         <v>2.7142857142857144</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <f>AVERAGE(F3:F9)</f>
         <v>3.5714285714285716</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="22">
+      <c r="G20" s="22"/>
+      <c r="H20" s="21">
         <f>AVERAGE(H3:H18)</f>
         <v>3.25</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="21">
         <f>AVERAGE(I3:I18)</f>
         <v>3.9375</v>
       </c>
@@ -4905,39 +4922,39 @@
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="37">
         <f>_xlfn.STDEV.S(B3:B9)</f>
         <v>0.97590007294853265</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="37">
         <f>_xlfn.STDEV.S(C3:C9)</f>
         <v>1.2535663410560176</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="23">
+      <c r="D21" s="22"/>
+      <c r="E21" s="37">
         <f>_xlfn.STDEV.S(E3:E9)</f>
         <v>1.3801311186847085</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="37">
         <f>_xlfn.STDEV.S(F3:F9)</f>
         <v>0.97590007294853265</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="23">
+      <c r="G21" s="22"/>
+      <c r="H21" s="37">
         <f>_xlfn.STDEV.S(H3:H18)</f>
         <v>1.390443574307614</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="37">
         <f>_xlfn.STDEV.S(I3:I18)</f>
         <v>1.0626225419530053</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
@@ -4951,55 +4968,60 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <f>_xlfn.T.TEST(E3:E11,H3:H16,1,2)</f>
-        <v>0.23227337599304232</v>
-      </c>
-      <c r="B25" s="18">
-        <f>_xlfn.T.TEST(B3:B11,H3:H16,1,2)</f>
-        <v>0.28564191552220131</v>
-      </c>
-      <c r="C25" s="19">
-        <f>_xlfn.T.TEST(B3:B11,E3:E11,1,1)</f>
+      <c r="A25" s="28">
+        <f>_xlfn.T.TEST(E3:E9,H3:H18,1,2)</f>
+        <v>0.20191087415133357</v>
+      </c>
+      <c r="B25" s="16">
+        <f>_xlfn.T.TEST(B3:B9,H3:H18,1,2)</f>
+        <v>0.29349633391942803</v>
+      </c>
+      <c r="C25" s="16">
+        <f>_xlfn.T.TEST(B3:B9,E3:E9,1,1)</f>
         <v>0.11241091070223835</v>
       </c>
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="11"/>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+    </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <f>_xlfn.T.TEST(I3:I16,F3:F11,1,3)</f>
-        <v>0.14642480944749009</v>
-      </c>
-      <c r="B30" s="17">
-        <f>_xlfn.T.TEST(I3:I16,C3:C11,1,3)</f>
-        <v>1.5885186880404776E-2</v>
-      </c>
-      <c r="C30" s="15">
-        <f>_xlfn.T.TEST(C3:C11,F3:F11,1,1)</f>
+      <c r="A30" s="28">
+        <f>_xlfn.T.TEST(I3:I18,F3:F9,1,3)</f>
+        <v>0.21784498807176245</v>
+      </c>
+      <c r="B30" s="16">
+        <f>_xlfn.T.TEST(I3:I18,C3:C9,1,3)</f>
+        <v>2.4049482754317945E-2</v>
+      </c>
+      <c r="C30" s="16">
+        <f>_xlfn.T.TEST(C3:C9,F3:F9,1,1)</f>
         <v>0.1704848063365802</v>
       </c>
     </row>
@@ -5020,8 +5042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,18 +5052,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="27"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5076,10 +5098,10 @@
       <c r="F3" s="5">
         <v>3</v>
       </c>
-      <c r="H3" s="21">
-        <v>4</v>
-      </c>
-      <c r="I3" s="21">
+      <c r="H3" s="19">
+        <v>4</v>
+      </c>
+      <c r="I3" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5096,10 +5118,10 @@
       <c r="F4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="21">
-        <v>5</v>
-      </c>
-      <c r="I4" s="21">
+      <c r="H4" s="19">
+        <v>5</v>
+      </c>
+      <c r="I4" s="19">
         <v>5</v>
       </c>
     </row>
@@ -5116,10 +5138,10 @@
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="H5" s="21">
-        <v>2</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="H5" s="19">
+        <v>2</v>
+      </c>
+      <c r="I5" s="19">
         <v>2</v>
       </c>
     </row>
@@ -5136,10 +5158,10 @@
       <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="H6" s="21">
-        <v>5</v>
-      </c>
-      <c r="I6" s="21">
+      <c r="H6" s="19">
+        <v>5</v>
+      </c>
+      <c r="I6" s="19">
         <v>5</v>
       </c>
     </row>
@@ -5156,10 +5178,10 @@
       <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="21">
-        <v>5</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="19">
         <v>5</v>
       </c>
     </row>
@@ -5176,10 +5198,10 @@
       <c r="F8" s="5">
         <v>4</v>
       </c>
-      <c r="H8" s="21">
-        <v>4</v>
-      </c>
-      <c r="I8" s="21">
+      <c r="H8" s="19">
+        <v>4</v>
+      </c>
+      <c r="I8" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5196,10 +5218,10 @@
       <c r="F9" s="5">
         <v>4</v>
       </c>
-      <c r="H9" s="21">
-        <v>3</v>
-      </c>
-      <c r="I9" s="21">
+      <c r="H9" s="19">
+        <v>3</v>
+      </c>
+      <c r="I9" s="19">
         <v>3</v>
       </c>
     </row>
@@ -5211,10 +5233,10 @@
       <c r="C10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="H10" s="21">
-        <v>4</v>
-      </c>
-      <c r="I10" s="21">
+      <c r="H10" s="19">
+        <v>4</v>
+      </c>
+      <c r="I10" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5226,66 +5248,66 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="H11" s="21">
-        <v>4</v>
-      </c>
-      <c r="I11" s="21">
+      <c r="H11" s="19">
+        <v>4</v>
+      </c>
+      <c r="I11" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="21">
-        <v>2</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="H12" s="19">
+        <v>2</v>
+      </c>
+      <c r="I12" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="21">
-        <v>5</v>
-      </c>
-      <c r="I13" s="21">
+      <c r="H13" s="19">
+        <v>5</v>
+      </c>
+      <c r="I13" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="21">
-        <v>5</v>
-      </c>
-      <c r="I14" s="21">
+      <c r="H14" s="19">
+        <v>5</v>
+      </c>
+      <c r="I14" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="21">
-        <v>4</v>
-      </c>
-      <c r="I15" s="21">
+      <c r="H15" s="19">
+        <v>4</v>
+      </c>
+      <c r="I15" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="21">
-        <v>1</v>
-      </c>
-      <c r="I16" s="21">
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="21">
-        <v>3</v>
-      </c>
-      <c r="I17" s="21">
+      <c r="H17" s="19">
+        <v>3</v>
+      </c>
+      <c r="I17" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="21">
-        <v>3</v>
-      </c>
-      <c r="I18" s="21">
+      <c r="H18" s="19">
+        <v>3</v>
+      </c>
+      <c r="I18" s="19">
         <v>3</v>
       </c>
     </row>
@@ -5293,29 +5315,29 @@
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <f>AVERAGE(B3:B10)</f>
         <v>2.5416666666666665</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <f>AVERAGE(C3:C10)</f>
         <v>3.8571428571428572</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="22">
+      <c r="D20" s="34"/>
+      <c r="E20" s="21">
         <f>AVERAGE(E3:E10)</f>
         <v>3.1428571428571428</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <f>AVERAGE(F3:F10)</f>
         <v>2.5714285714285716</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="22">
+      <c r="G20" s="34"/>
+      <c r="H20" s="21">
         <f>AVERAGE(H3:H18)</f>
         <v>3.6875</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="21">
         <f>AVERAGE(I3:I18)</f>
         <v>3.6875</v>
       </c>
@@ -5324,39 +5346,39 @@
       <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="35">
         <f>_xlfn.STDEV.S(B3:B10)</f>
         <v>1.622632585626367</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="35">
         <f>_xlfn.STDEV.S(C3:C10)</f>
         <v>0.89973541084243769</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25">
+      <c r="D21" s="36"/>
+      <c r="E21" s="35">
         <f>_xlfn.STDEV.S(E3:E10)</f>
         <v>1.2149857925879122</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="35">
         <f>_xlfn.STDEV.S(F3:F10)</f>
         <v>1.1338934190276817</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="25">
+      <c r="G21" s="36"/>
+      <c r="H21" s="35">
         <f>_xlfn.STDEV.S(H3:H18)</f>
         <v>1.25</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="35">
         <f>_xlfn.STDEV.S(I3:I18)</f>
         <v>1.25</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
@@ -5370,16 +5392,16 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <f>_xlfn.T.TEST(E3:E11,H3:H16,1,2)</f>
-        <v>0.14607858069301433</v>
-      </c>
-      <c r="B25" s="18">
-        <f>_xlfn.T.TEST(B3:B11,H3:H16,1,2)</f>
-        <v>3.1694908147270953E-2</v>
-      </c>
-      <c r="C25" s="19">
-        <f>_xlfn.T.TEST(B3:B11,E3:E11,1,1)</f>
+      <c r="A25" s="13">
+        <f>_xlfn.T.TEST(E3:E9,H3:H18,1,2)</f>
+        <v>0.17174482161962717</v>
+      </c>
+      <c r="B25" s="16">
+        <f>_xlfn.T.TEST(B3:B9,H3:H18,1,2)</f>
+        <v>8.8977817353883382E-2</v>
+      </c>
+      <c r="C25" s="17">
+        <f>_xlfn.T.TEST(B3:B9,E3:E9,1,1)</f>
         <v>0.37224633221277204</v>
       </c>
     </row>
@@ -5389,11 +5411,11 @@
       <c r="C26" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -5407,15 +5429,15 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <f>_xlfn.T.TEST(I3:I16,F3:F11,1,3)</f>
-        <v>2.2934105052452206E-2</v>
-      </c>
-      <c r="B30" s="18">
-        <f>_xlfn.T.TEST(I3:I16,C3:C11,1,3)</f>
-        <v>0.30788443184136399</v>
-      </c>
-      <c r="C30" s="18">
+      <c r="A30" s="13">
+        <f>_xlfn.T.TEST(I3:I18,F3:F9,1,3)</f>
+        <v>2.7984686549191982E-2</v>
+      </c>
+      <c r="B30" s="16">
+        <f>_xlfn.T.TEST(I3:I18,C3:C9,1,3)</f>
+        <v>0.35911670332736345</v>
+      </c>
+      <c r="C30" s="16">
         <f>_xlfn.T.TEST(C3:C11,F3:F11,1,1)</f>
         <v>6.0976210691944033E-2</v>
       </c>
@@ -5437,25 +5459,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:I21"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="27"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5490,10 +5512,10 @@
       <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="21">
-        <v>5</v>
-      </c>
-      <c r="I3" s="21">
+      <c r="H3" s="19">
+        <v>5</v>
+      </c>
+      <c r="I3" s="19">
         <v>3</v>
       </c>
     </row>
@@ -5510,10 +5532,10 @@
       <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="H4" s="21">
-        <v>5</v>
-      </c>
-      <c r="I4" s="21">
+      <c r="H4" s="19">
+        <v>5</v>
+      </c>
+      <c r="I4" s="19">
         <v>2</v>
       </c>
     </row>
@@ -5530,10 +5552,10 @@
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="H5" s="21">
-        <v>4</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="H5" s="19">
+        <v>4</v>
+      </c>
+      <c r="I5" s="19">
         <v>2</v>
       </c>
     </row>
@@ -5550,10 +5572,10 @@
       <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="H6" s="21">
-        <v>5</v>
-      </c>
-      <c r="I6" s="21">
+      <c r="H6" s="19">
+        <v>5</v>
+      </c>
+      <c r="I6" s="19">
         <v>1</v>
       </c>
     </row>
@@ -5570,10 +5592,10 @@
       <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="21">
-        <v>5</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5590,10 +5612,10 @@
       <c r="F8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="21">
-        <v>4</v>
-      </c>
-      <c r="I8" s="21">
+      <c r="H8" s="19">
+        <v>4</v>
+      </c>
+      <c r="I8" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5610,10 +5632,10 @@
       <c r="F9" s="5">
         <v>5</v>
       </c>
-      <c r="H9" s="21">
-        <v>5</v>
-      </c>
-      <c r="I9" s="21">
+      <c r="H9" s="19">
+        <v>5</v>
+      </c>
+      <c r="I9" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5622,10 +5644,10 @@
       <c r="C10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="H10" s="21">
-        <v>5</v>
-      </c>
-      <c r="I10" s="21">
+      <c r="H10" s="19">
+        <v>5</v>
+      </c>
+      <c r="I10" s="19">
         <v>4</v>
       </c>
     </row>
@@ -5634,100 +5656,100 @@
       <c r="C11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="H11" s="21">
-        <v>2</v>
-      </c>
-      <c r="I11" s="21">
+      <c r="H11" s="19">
+        <v>2</v>
+      </c>
+      <c r="I11" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="21">
-        <v>1</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="H12" s="19">
+        <v>1</v>
+      </c>
+      <c r="I12" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="21">
-        <v>2</v>
-      </c>
-      <c r="I13" s="21">
+      <c r="H13" s="19">
+        <v>2</v>
+      </c>
+      <c r="I13" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="21">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21">
+      <c r="H14" s="19">
+        <v>1</v>
+      </c>
+      <c r="I14" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="21">
-        <v>5</v>
-      </c>
-      <c r="I15" s="21">
+      <c r="H15" s="19">
+        <v>5</v>
+      </c>
+      <c r="I15" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="21">
-        <v>3</v>
-      </c>
-      <c r="I16" s="21">
+      <c r="H16" s="19">
+        <v>3</v>
+      </c>
+      <c r="I16" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="21">
-        <v>2</v>
-      </c>
-      <c r="I17" s="21">
+      <c r="H17" s="19">
+        <v>2</v>
+      </c>
+      <c r="I17" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="21">
-        <v>2</v>
-      </c>
-      <c r="I18" s="21">
+      <c r="H18" s="19">
+        <v>2</v>
+      </c>
+      <c r="I18" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="21">
         <f>AVERAGE(B3:B9)</f>
         <v>4.4285714285714288</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="21">
         <f>AVERAGE(C3:C9)</f>
         <v>3.1428571428571428</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="32">
+      <c r="D21" s="22"/>
+      <c r="E21" s="21">
         <f>AVERAGE(E3:E9)</f>
         <v>2.1428571428571428</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="21">
         <f>AVERAGE(F3:F9)</f>
         <v>2.4285714285714284</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="32">
+      <c r="G21" s="22"/>
+      <c r="H21" s="21">
         <f>AVERAGE(H3:H18)</f>
         <v>3.5</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="21">
         <f>AVERAGE(I3:I18)</f>
         <v>3.375</v>
       </c>
@@ -5736,39 +5758,39 @@
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="20">
         <f>_xlfn.STDEV.S(B3:B9)</f>
         <v>0.78679579246944398</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="20">
         <f>_xlfn.STDEV.S(C3:C9)</f>
         <v>1.0690449676496978</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="23">
+      <c r="E22" s="20">
         <f>_xlfn.STDEV.S(E3:E10)</f>
         <v>0.89973541084243702</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <f>_xlfn.STDEV.S(F3:F9)</f>
         <v>1.2724180205607036</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="23">
+      <c r="H22" s="20">
         <f>_xlfn.STDEV.S(H3:H18)</f>
         <v>1.5916448515084429</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="20">
         <f>_xlfn.STDEV.S(I3:I18)</f>
         <v>1.3601470508735443</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
@@ -5782,15 +5804,15 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
-        <f>_xlfn.T.TEST(E3:E11,H3:H16,1,2)</f>
-        <v>1.3140899885154541E-2</v>
-      </c>
-      <c r="B26" s="18">
-        <f>_xlfn.T.TEST(B3:B11,H3:H16,1,2)</f>
-        <v>0.13996454157555172</v>
-      </c>
-      <c r="C26" s="16">
+      <c r="A26" s="12">
+        <f>_xlfn.T.TEST(E3:E9,H3:H18,1,2)</f>
+        <v>2.4170437676663253E-2</v>
+      </c>
+      <c r="B26" s="16">
+        <f>_xlfn.T.TEST(B3:B9,H3:H18,1,2)</f>
+        <v>8.0381656058486448E-2</v>
+      </c>
+      <c r="C26" s="14">
         <f>_xlfn.T.TEST(B3:B11,E3:E11,1,1)</f>
         <v>4.6376272408676956E-3</v>
       </c>
@@ -5801,11 +5823,11 @@
       <c r="C27" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -5819,15 +5841,15 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <f>_xlfn.T.TEST(I3:I16,F3:F11,1,3)</f>
-        <v>3.9839828482185924E-2</v>
-      </c>
-      <c r="B31" s="17">
-        <f>_xlfn.T.TEST(I3:I16,C3:C11,1,3)</f>
-        <v>0.2200737300200426</v>
-      </c>
-      <c r="C31" s="16">
+      <c r="A31" s="13">
+        <f>_xlfn.T.TEST(I3:I18,F3:F9,1,3)</f>
+        <v>6.674927474552074E-2</v>
+      </c>
+      <c r="B31" s="15">
+        <f>_xlfn.T.TEST(I3:I18,C3:C9,1,3)</f>
+        <v>0.33334270535289157</v>
+      </c>
+      <c r="C31" s="14">
         <f>_xlfn.T.TEST(C3:C11,F3:F11,1,1)</f>
         <v>0.2053870232364105</v>
       </c>

</xml_diff>